<commit_message>
replaced ebi-a-GCST003374/Chronic kidney disease with ieu-a-1102/Chronic kidney disease (these are the same studies but the PRS for CKD was based on ieu-a-1102)
replaced ebi-a-GCST005047/type2 diabetes with ieu-a-26/type 2 diabetes (these are the same studies but the PRS for T2D was based on ieu-a-26)

replaced ieu-a-1024/MS with ieu-b-18/MS (the PRS was based on ieu-b-18; these are different studies)

removed ieu-a-986/LC in never smokers (not in PRS analysis)

removed ieu-a-988/small cell lung cancer (not in PRS analysis)

removed the following traits: HDLc, LDLc, Total cholesterol, Triglycerides, Systolic blood pressure, Diastolic blood pressure, Cancer code  self-reported: squamous cell carcinoma,
Type of cancer: ICD10: C64 Malignant neoplasm of kidney, except renal pelvis, Cancer code, self-reported: basal cell carcinoma
</commit_message>
<xml_diff>
--- a/data/Supplementary_Table5.xlsx
+++ b/data/Supplementary_Table5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ph14916/ukbb-prot-prs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F0A2DC-A284-0344-8212-6277FC955AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2713E16-FAA3-524E-AF92-B361F5A5B8D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19960" xr2:uid="{05F3420C-F508-254F-A908-4F7C3F1B436E}"/>
   </bookViews>
@@ -545,10 +545,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -869,7 +869,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>